<commit_message>
Working on exemplar table.
</commit_message>
<xml_diff>
--- a/inst/extdata/Exemplar_Table.xlsx
+++ b/inst/extdata/Exemplar_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/SEAPSUTWorkflow/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/Dropbox/Fellowship 1960-2015 PFU database/Database plan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8677A4E8-0ED6-E74B-A897-8EBD3274EAB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C2A668-EED4-6743-B21F-3C1055EF4A31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="37800" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23240" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exemplar_table" sheetId="5" r:id="rId1"/>
@@ -23,14 +23,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">exemplar_table!$A$1:$BA$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1360,9 +1352,6 @@
     <t>Data for Eritrea are available from 1992. Prior to that, they are included in Ethiopia</t>
   </si>
   <si>
-    <t>Former Yugoslavia (Split 27/04/1992). Before 1990, includes Bosnia and Herzegovina; Croatia; Republic of North Macedonia (North Macedonia); Kosovo; Montenegro; Slovenia and Serbia.</t>
-  </si>
-  <si>
     <t>Data for Mongolia are available starting in 1985. Prior to that, they are included in Other Asia.</t>
   </si>
   <si>
@@ -1396,21 +1385,6 @@
     <t xml:space="preserve">Hi Matt, here's my proposed code structure! Apologies if it is incorrect, my R skills are very much a work in progress.  </t>
   </si>
   <si>
-    <t>Rank_TFC_2017i</t>
-  </si>
-  <si>
-    <t>Region_Code</t>
-  </si>
-  <si>
-    <t>ROW_Code</t>
-  </si>
-  <si>
-    <t>Countries_or_Group</t>
-  </si>
-  <si>
-    <t>Exemplar_Country</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aim: To allocate the country names/3-letter ISO codes to either: 1) a ROW region, or 2) the appropriate country code for a particular year as defined in the IEA WEEB 2019 database documentation. </t>
   </si>
   <si>
@@ -1423,16 +1397,34 @@
     <t>Restofworld</t>
   </si>
   <si>
-    <t>Former Soviet Union (Split 26 Novemeber 1991) Before 1990, includes Armenia; Azerbaijan; Belarus; Estonia; Georgia; Kazakhstan; Kyrgyzstan; Latvia; Lithuania; Republic of Moldova; Russian Federation; Tajikistan; Turkmenistan; Ukraine and Uzbekistan.</t>
-  </si>
-  <si>
     <t>Former Czech and Slovak Federative Republic (01 January 1993)</t>
   </si>
   <si>
     <t>South Sudan and Sudan (Split 09 July 2011) Data for South Sudan are available from 2012. Prior to 2012, they are included in Sudan.</t>
   </si>
   <si>
-    <t>Individual, Restofworld, FSU, YGS</t>
+    <t>Former Soviet Union (Split 26 Novemeber 1991)  Data before 1990, includes Armenia; Azerbaijan; Belarus; Estonia; Georgia; Kazakhstan; Kyrgyzstan; Latvia; Lithuania; Republic of Moldova; Russian Federation; Tajikistan; Turkmenistan; Ukraine and Uzbekistan.</t>
+  </si>
+  <si>
+    <t>Former Yugoslavia (Split 27/04/1992). Data before 1990, includes Bosnia and Herzegovina; Croatia; Republic of North Macedonia (North Macedonia); Kosovo; Montenegro; Slovenia and Serbia.</t>
+  </si>
+  <si>
+    <t>ROW.code</t>
+  </si>
+  <si>
+    <t>Exemplar.country</t>
+  </si>
+  <si>
+    <t>Country.name</t>
+  </si>
+  <si>
+    <t>Region.code</t>
+  </si>
+  <si>
+    <t>Aggregation</t>
+  </si>
+  <si>
+    <t>Rank.TFC.2017i</t>
   </si>
 </sst>
 </file>
@@ -3108,9 +3100,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BA151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z1" sqref="Z1:Z1048576"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3126,22 +3118,22 @@
   <sheetData>
     <row r="1" spans="1:53" s="24" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>454</v>
+        <v>463</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="G1" s="14">
         <v>1971</v>
@@ -3290,7 +3282,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>390</v>
@@ -3302,7 +3294,7 @@
         <v>265</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>45</v>
@@ -3451,7 +3443,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>391</v>
@@ -3463,7 +3455,7 @@
         <v>249</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>250</v>
@@ -3612,7 +3604,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>390</v>
@@ -3624,7 +3616,7 @@
         <v>102</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>103</v>
@@ -3785,7 +3777,7 @@
         <v>198</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>290</v>
@@ -3934,7 +3926,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>390</v>
@@ -3946,7 +3938,7 @@
         <v>117</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>118</v>
@@ -4095,7 +4087,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>391</v>
@@ -4107,7 +4099,7 @@
         <v>31</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>32</v>
@@ -4256,7 +4248,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>392</v>
@@ -4268,7 +4260,7 @@
         <v>84</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>85</v>
@@ -4417,7 +4409,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>391</v>
@@ -4429,7 +4421,7 @@
         <v>41</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>42</v>
@@ -4578,7 +4570,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>390</v>
@@ -4590,7 +4582,7 @@
         <v>272</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>106</v>
@@ -4739,7 +4731,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>390</v>
@@ -4751,7 +4743,7 @@
         <v>273</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>126</v>
@@ -4900,7 +4892,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>390</v>
@@ -4912,7 +4904,7 @@
         <v>104</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>105</v>
@@ -5061,7 +5053,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>392</v>
@@ -5073,7 +5065,7 @@
         <v>78</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>79</v>
@@ -5222,7 +5214,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>390</v>
@@ -5234,7 +5226,7 @@
         <v>200</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>201</v>
@@ -5383,7 +5375,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>391</v>
@@ -5395,7 +5387,7 @@
         <v>174</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>175</v>
@@ -5544,7 +5536,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>392</v>
@@ -5556,7 +5548,7 @@
         <v>247</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>248</v>
@@ -5705,7 +5697,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>391</v>
@@ -5717,7 +5709,7 @@
         <v>148</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>149</v>
@@ -5866,7 +5858,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>392</v>
@@ -5878,7 +5870,7 @@
         <v>113</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>114</v>
@@ -6027,7 +6019,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>390</v>
@@ -6039,7 +6031,7 @@
         <v>239</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>240</v>
@@ -6188,7 +6180,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>390</v>
@@ -6200,7 +6192,7 @@
         <v>231</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>232</v>
@@ -6349,7 +6341,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>390</v>
@@ -6361,7 +6353,7 @@
         <v>180</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>181</v>
@@ -6510,7 +6502,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>392</v>
@@ -6522,7 +6514,7 @@
         <v>213</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>214</v>
@@ -6671,19 +6663,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>393</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>11</v>
@@ -6832,7 +6824,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>392</v>
@@ -6844,7 +6836,7 @@
         <v>190</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>191</v>
@@ -6993,7 +6985,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>390</v>
@@ -7005,7 +6997,7 @@
         <v>278</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>227</v>
@@ -7154,7 +7146,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>389</v>
@@ -7166,7 +7158,7 @@
         <v>211</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>212</v>
@@ -7315,7 +7307,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>389</v>
@@ -7327,7 +7319,7 @@
         <v>337</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G27" s="13" t="s">
         <v>366</v>
@@ -7476,7 +7468,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>390</v>
@@ -7488,7 +7480,7 @@
         <v>256</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>257</v>
@@ -7637,7 +7629,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>391</v>
@@ -7649,7 +7641,7 @@
         <v>6</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>7</v>
@@ -7798,7 +7790,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>389</v>
@@ -7810,7 +7802,7 @@
         <v>66</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>67</v>
@@ -7959,7 +7951,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>390</v>
@@ -7971,7 +7963,7 @@
         <v>142</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>143</v>
@@ -8120,7 +8112,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>392</v>
@@ -8132,7 +8124,7 @@
         <v>165</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>166</v>
@@ -8281,7 +8273,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>390</v>
@@ -8293,7 +8285,7 @@
         <v>245</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>246</v>
@@ -8454,7 +8446,7 @@
         <v>243</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>290</v>
@@ -8603,7 +8595,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C35" s="17" t="s">
         <v>392</v>
@@ -8615,7 +8607,7 @@
         <v>22</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>23</v>
@@ -8776,7 +8768,7 @@
         <v>121</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>290</v>
@@ -8925,7 +8917,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>389</v>
@@ -8937,7 +8929,7 @@
         <v>74</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>75</v>
@@ -9086,7 +9078,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C38" s="18" t="s">
         <v>389</v>
@@ -9098,7 +9090,7 @@
         <v>2</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>3</v>
@@ -9247,7 +9239,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C39" s="18" t="s">
         <v>392</v>
@@ -9259,7 +9251,7 @@
         <v>221</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>222</v>
@@ -9408,7 +9400,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>390</v>
@@ -9420,7 +9412,7 @@
         <v>188</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>189</v>
@@ -9569,7 +9561,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>390</v>
@@ -9581,7 +9573,7 @@
         <v>18</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>19</v>
@@ -9730,7 +9722,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C42" s="18" t="s">
         <v>391</v>
@@ -9742,7 +9734,7 @@
         <v>280</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>255</v>
@@ -9891,7 +9883,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>391</v>
@@ -9903,7 +9895,7 @@
         <v>46</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>47</v>
@@ -10052,7 +10044,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C44" s="18" t="s">
         <v>392</v>
@@ -10064,7 +10056,7 @@
         <v>12</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>13</v>
@@ -10213,7 +10205,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C45" s="18" t="s">
         <v>392</v>
@@ -10225,7 +10217,7 @@
         <v>58</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>59</v>
@@ -10374,7 +10366,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C46" s="18" t="s">
         <v>391</v>
@@ -10386,7 +10378,7 @@
         <v>43</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>44</v>
@@ -10535,7 +10527,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C47" s="18" t="s">
         <v>392</v>
@@ -10547,7 +10539,7 @@
         <v>76</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>77</v>
@@ -10696,7 +10688,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C48" s="18" t="s">
         <v>389</v>
@@ -10708,7 +10700,7 @@
         <v>270</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>48</v>
@@ -10857,7 +10849,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C49" s="18" t="s">
         <v>390</v>
@@ -10869,7 +10861,7 @@
         <v>206</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>207</v>
@@ -11018,7 +11010,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C50" s="18" t="s">
         <v>392</v>
@@ -11030,7 +11022,7 @@
         <v>196</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>197</v>
@@ -11191,7 +11183,7 @@
         <v>253</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>290</v>
@@ -11340,7 +11332,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C52" s="17" t="s">
         <v>390</v>
@@ -11352,7 +11344,7 @@
         <v>178</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>179</v>
@@ -11501,7 +11493,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C53" s="17" t="s">
         <v>392</v>
@@ -11513,7 +11505,7 @@
         <v>176</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>177</v>
@@ -11662,7 +11654,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C54" s="17" t="s">
         <v>390</v>
@@ -11674,7 +11666,7 @@
         <v>107</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>108</v>
@@ -11823,7 +11815,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C55" s="17" t="s">
         <v>392</v>
@@ -11835,7 +11827,7 @@
         <v>98</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>99</v>
@@ -11984,7 +11976,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C56" s="17" t="s">
         <v>390</v>
@@ -11996,7 +11988,7 @@
         <v>159</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>160</v>
@@ -12145,7 +12137,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C57" s="17" t="s">
         <v>390</v>
@@ -12157,7 +12149,7 @@
         <v>127</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>128</v>
@@ -12306,7 +12298,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C58" s="17" t="s">
         <v>391</v>
@@ -12318,7 +12310,7 @@
         <v>186</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>187</v>
@@ -12479,7 +12471,7 @@
         <v>20</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>290</v>
@@ -12628,7 +12620,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C60" s="18" t="s">
         <v>392</v>
@@ -12640,7 +12632,7 @@
         <v>223</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>224</v>
@@ -12789,7 +12781,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C61" s="18" t="s">
         <v>390</v>
@@ -12801,7 +12793,7 @@
         <v>194</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>195</v>
@@ -12962,7 +12954,7 @@
         <v>241</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>290</v>
@@ -13111,7 +13103,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C63" s="18" t="s">
         <v>389</v>
@@ -13123,7 +13115,7 @@
         <v>279</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>230</v>
@@ -13272,7 +13264,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C64" s="18" t="s">
         <v>389</v>
@@ -13284,7 +13276,7 @@
         <v>123</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>124</v>
@@ -13433,7 +13425,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C65" s="18" t="s">
         <v>392</v>
@@ -13445,7 +13437,7 @@
         <v>90</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>91</v>
@@ -13594,7 +13586,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C66" s="18" t="s">
         <v>392</v>
@@ -13606,7 +13598,7 @@
         <v>192</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>193</v>
@@ -13755,7 +13747,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C67" s="18" t="s">
         <v>389</v>
@@ -13767,7 +13759,7 @@
         <v>155</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>156</v>
@@ -13916,7 +13908,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C68" s="18" t="s">
         <v>390</v>
@@ -13928,7 +13920,7 @@
         <v>111</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>112</v>
@@ -14077,19 +14069,19 @@
         <v>68</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C69" s="18" t="s">
         <v>393</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>168</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>169</v>
@@ -14238,7 +14230,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C70" s="16" t="s">
         <v>390</v>
@@ -14250,7 +14242,7 @@
         <v>339</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G70" s="13" t="s">
         <v>368</v>
@@ -14399,7 +14391,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C71" s="18" t="s">
         <v>392</v>
@@ -14411,7 +14403,7 @@
         <v>60</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>61</v>
@@ -14560,7 +14552,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C72" s="18" t="s">
         <v>390</v>
@@ -14572,7 +14564,7 @@
         <v>163</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>164</v>
@@ -14721,7 +14713,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C73" s="18" t="s">
         <v>389</v>
@@ -14733,7 +14725,7 @@
         <v>217</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>218</v>
@@ -14882,7 +14874,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C74" s="18" t="s">
         <v>391</v>
@@ -14894,7 +14886,7 @@
         <v>64</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>65</v>
@@ -15043,7 +15035,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C75" s="18" t="s">
         <v>391</v>
@@ -15055,7 +15047,7 @@
         <v>235</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>236</v>
@@ -15204,7 +15196,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C76" s="18" t="s">
         <v>391</v>
@@ -15216,7 +15208,7 @@
         <v>92</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>93</v>
@@ -15365,7 +15357,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C77" s="18" t="s">
         <v>392</v>
@@ -15377,7 +15369,7 @@
         <v>276</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>208</v>
@@ -15526,7 +15518,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C78" s="18" t="s">
         <v>392</v>
@@ -15538,7 +15530,7 @@
         <v>109</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>110</v>
@@ -15687,7 +15679,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C79" s="18" t="s">
         <v>390</v>
@@ -15699,7 +15691,7 @@
         <v>215</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>216</v>
@@ -15848,7 +15840,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C80" s="18" t="s">
         <v>392</v>
@@ -15860,7 +15852,7 @@
         <v>35</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>36</v>
@@ -16009,7 +16001,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C81" s="18" t="s">
         <v>389</v>
@@ -16021,7 +16013,7 @@
         <v>262</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>263</v>
@@ -16170,7 +16162,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C82" s="18" t="s">
         <v>389</v>
@@ -16182,7 +16174,7 @@
         <v>4</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>5</v>
@@ -16331,7 +16323,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C83" s="18" t="s">
         <v>389</v>
@@ -16343,7 +16335,7 @@
         <v>260</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>261</v>
@@ -16504,7 +16496,7 @@
         <v>204</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>289</v>
@@ -16653,7 +16645,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C85" s="18" t="s">
         <v>389</v>
@@ -16665,7 +16657,7 @@
         <v>345</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>364</v>
@@ -16826,7 +16818,7 @@
         <v>14</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>290</v>
@@ -16975,7 +16967,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C87" s="18" t="s">
         <v>389</v>
@@ -16987,7 +16979,7 @@
         <v>136</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>135</v>
@@ -17136,7 +17128,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C88" s="18" t="s">
         <v>389</v>
@@ -17148,7 +17140,7 @@
         <v>237</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G88" s="2" t="s">
         <v>238</v>
@@ -17297,7 +17289,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C89" s="18" t="s">
         <v>391</v>
@@ -17309,7 +17301,7 @@
         <v>54</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>55</v>
@@ -17458,7 +17450,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C90" s="18" t="s">
         <v>391</v>
@@ -17470,7 +17462,7 @@
         <v>264</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>26</v>
@@ -17619,7 +17611,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C91" s="18" t="s">
         <v>389</v>
@@ -17631,7 +17623,7 @@
         <v>39</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>40</v>
@@ -17792,7 +17784,7 @@
         <v>52</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>289</v>
@@ -17941,7 +17933,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C93" s="18" t="s">
         <v>389</v>
@@ -17953,7 +17945,7 @@
         <v>267</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>51</v>
@@ -18102,7 +18094,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C94" s="18" t="s">
         <v>389</v>
@@ -18114,7 +18106,7 @@
         <v>86</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>87</v>
@@ -18263,7 +18255,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C95" s="18" t="s">
         <v>390</v>
@@ -18275,7 +18267,7 @@
         <v>37</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G95" s="2" t="s">
         <v>368</v>
@@ -18424,7 +18416,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C96" s="18" t="s">
         <v>390</v>
@@ -18436,7 +18428,7 @@
         <v>119</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>120</v>
@@ -18597,7 +18589,7 @@
         <v>137</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G97" s="2" t="s">
         <v>290</v>
@@ -18746,7 +18738,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C98" s="18" t="s">
         <v>391</v>
@@ -18758,7 +18750,7 @@
         <v>184</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G98" s="2" t="s">
         <v>185</v>
@@ -18907,7 +18899,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C99" s="18" t="s">
         <v>390</v>
@@ -18919,7 +18911,7 @@
         <v>16</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>17</v>
@@ -19068,7 +19060,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C100" s="18" t="s">
         <v>391</v>
@@ -19080,7 +19072,7 @@
         <v>62</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>63</v>
@@ -19229,7 +19221,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C101" s="18" t="s">
         <v>390</v>
@@ -19241,7 +19233,7 @@
         <v>269</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>125</v>
@@ -19390,7 +19382,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C102" s="18" t="s">
         <v>389</v>
@@ -19402,7 +19394,7 @@
         <v>157</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G102" s="2" t="s">
         <v>158</v>
@@ -19551,7 +19543,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C103" s="18" t="s">
         <v>390</v>
@@ -19563,7 +19555,7 @@
         <v>133</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G103" s="2" t="s">
         <v>134</v>
@@ -19712,7 +19704,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C104" s="18" t="s">
         <v>390</v>
@@ -19724,7 +19716,7 @@
         <v>225</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G104" s="2" t="s">
         <v>226</v>
@@ -19873,7 +19865,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C105" s="18" t="s">
         <v>391</v>
@@ -19885,7 +19877,7 @@
         <v>96</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G105" s="2" t="s">
         <v>97</v>
@@ -20046,7 +20038,7 @@
         <v>209</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G106" s="2" t="s">
         <v>289</v>
@@ -20195,7 +20187,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C107" s="18" t="s">
         <v>391</v>
@@ -20207,7 +20199,7 @@
         <v>251</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G107" s="2" t="s">
         <v>252</v>
@@ -20356,7 +20348,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C108" s="18" t="s">
         <v>389</v>
@@ -20368,7 +20360,7 @@
         <v>80</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G108" s="2" t="s">
         <v>81</v>
@@ -20529,7 +20521,7 @@
         <v>82</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G109" s="2" t="s">
         <v>290</v>
@@ -20678,7 +20670,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C110" s="18" t="s">
         <v>389</v>
@@ -20690,7 +20682,7 @@
         <v>24</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G110" s="2" t="s">
         <v>25</v>
@@ -20839,7 +20831,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C111" s="18" t="s">
         <v>391</v>
@@ -20851,7 +20843,7 @@
         <v>49</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G111" s="2" t="s">
         <v>50</v>
@@ -21012,7 +21004,7 @@
         <v>131</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G112" s="2" t="s">
         <v>290</v>
@@ -21161,7 +21153,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C113" s="17" t="s">
         <v>392</v>
@@ -21173,7 +21165,7 @@
         <v>139</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G113" s="2" t="s">
         <v>140</v>
@@ -21322,7 +21314,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C114" s="17" t="s">
         <v>391</v>
@@ -21334,7 +21326,7 @@
         <v>182</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G114" s="2" t="s">
         <v>183</v>
@@ -21495,7 +21487,7 @@
         <v>27</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G115" s="2" t="s">
         <v>289</v>
@@ -21656,7 +21648,7 @@
         <v>129</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G116" s="2" t="s">
         <v>290</v>
@@ -21805,7 +21797,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C117" s="17" t="s">
         <v>390</v>
@@ -21817,7 +21809,7 @@
         <v>151</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G117" s="2" t="s">
         <v>368</v>
@@ -21966,7 +21958,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C118" s="17" t="s">
         <v>391</v>
@@ -21978,7 +21970,7 @@
         <v>338</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G118" s="13" t="s">
         <v>367</v>
@@ -22127,7 +22119,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C119" s="17" t="s">
         <v>391</v>
@@ -22139,7 +22131,7 @@
         <v>94</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G119" s="2" t="s">
         <v>95</v>
@@ -22288,7 +22280,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C120" s="17" t="s">
         <v>389</v>
@@ -22300,7 +22292,7 @@
         <v>202</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G120" s="2" t="s">
         <v>203</v>
@@ -22461,7 +22453,7 @@
         <v>275</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G121" s="2" t="s">
         <v>290</v>
@@ -22610,7 +22602,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C122" s="16" t="s">
         <v>392</v>
@@ -22622,7 +22614,7 @@
         <v>100</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G122" s="2" t="s">
         <v>101</v>
@@ -22771,7 +22763,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C123" s="15" t="s">
         <v>392</v>
@@ -22783,7 +22775,7 @@
         <v>72</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G123" s="2" t="s">
         <v>290</v>
@@ -22932,7 +22924,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C124" s="17" t="s">
         <v>389</v>
@@ -22944,7 +22936,7 @@
         <v>172</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G124" s="2" t="s">
         <v>366</v>
@@ -23105,7 +23097,7 @@
         <v>228</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G125" s="2" t="s">
         <v>290</v>
@@ -23254,7 +23246,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C126" s="17" t="s">
         <v>391</v>
@@ -23266,7 +23258,7 @@
         <v>170</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G126" s="2" t="s">
         <v>171</v>
@@ -23415,7 +23407,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C127" s="17" t="s">
         <v>391</v>
@@ -23427,7 +23419,7 @@
         <v>68</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G127" s="2" t="s">
         <v>69</v>
@@ -23576,7 +23568,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C128" s="17" t="s">
         <v>389</v>
@@ -23588,7 +23580,7 @@
         <v>233</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G128" s="2" t="s">
         <v>234</v>
@@ -23737,7 +23729,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C129" s="17" t="s">
         <v>390</v>
@@ -23749,7 +23741,7 @@
         <v>258</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G129" s="2" t="s">
         <v>259</v>
@@ -23910,7 +23902,7 @@
         <v>8</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G130" s="2" t="s">
         <v>290</v>
@@ -24059,7 +24051,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C131" s="17" t="s">
         <v>392</v>
@@ -24071,7 +24063,7 @@
         <v>0</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G131" s="2" t="s">
         <v>1</v>
@@ -24220,7 +24212,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C132" s="18" t="s">
         <v>389</v>
@@ -24232,7 +24224,7 @@
         <v>29</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G132" s="2" t="s">
         <v>366</v>
@@ -24393,7 +24385,7 @@
         <v>271</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G133" s="2" t="s">
         <v>289</v>
@@ -24542,7 +24534,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C134" s="17" t="s">
         <v>389</v>
@@ -24554,7 +24546,7 @@
         <v>266</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G134" s="2" t="s">
         <v>48</v>
@@ -24703,7 +24695,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C135" s="17" t="s">
         <v>391</v>
@@ -24715,7 +24707,7 @@
         <v>115</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G135" s="2" t="s">
         <v>116</v>
@@ -24864,7 +24856,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C136" s="17" t="s">
         <v>389</v>
@@ -24876,7 +24868,7 @@
         <v>161</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G136" s="2" t="s">
         <v>366</v>
@@ -25025,7 +25017,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C137" s="17" t="s">
         <v>390</v>
@@ -25037,7 +25029,7 @@
         <v>344</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G137" s="2" t="s">
         <v>369</v>
@@ -25186,7 +25178,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C138" s="17" t="s">
         <v>390</v>
@@ -25198,7 +25190,7 @@
         <v>56</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G138" s="2" t="s">
         <v>57</v>
@@ -25359,7 +25351,7 @@
         <v>274</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G139" s="2" t="s">
         <v>289</v>
@@ -25508,7 +25500,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C140" s="17" t="s">
         <v>390</v>
@@ -25520,7 +25512,7 @@
         <v>33</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G140" s="2" t="s">
         <v>34</v>
@@ -25669,7 +25661,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C141" s="17" t="s">
         <v>389</v>
@@ -25681,7 +25673,7 @@
         <v>146</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G141" s="2" t="s">
         <v>147</v>
@@ -25842,7 +25834,7 @@
         <v>153</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G142" s="2" t="s">
         <v>289</v>
@@ -25991,7 +25983,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C143" s="18" t="s">
         <v>391</v>
@@ -26003,7 +25995,7 @@
         <v>268</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G143" s="2" t="s">
         <v>167</v>
@@ -26152,7 +26144,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C144" s="18" t="s">
         <v>391</v>
@@ -26164,7 +26156,7 @@
         <v>219</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G144" s="2" t="s">
         <v>367</v>
@@ -26313,7 +26305,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C145" s="18" t="s">
         <v>389</v>
@@ -26325,7 +26317,7 @@
         <v>70</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G145" s="2" t="s">
         <v>75</v>
@@ -26474,7 +26466,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C146" s="18" t="s">
         <v>392</v>
@@ -26486,7 +26478,7 @@
         <v>144</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G146" s="2" t="s">
         <v>145</v>
@@ -26635,7 +26627,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C147" s="18" t="s">
         <v>389</v>
@@ -26647,7 +26639,7 @@
         <v>277</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G147" s="2" t="s">
         <v>218</v>
@@ -26796,7 +26788,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C148" s="18" t="s">
         <v>392</v>
@@ -26808,7 +26800,7 @@
         <v>88</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G148" s="2" t="s">
         <v>89</v>
@@ -26957,7 +26949,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="18" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C149" s="17" t="s">
         <v>392</v>
@@ -26969,7 +26961,7 @@
         <v>341</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G149" s="2" t="s">
         <v>365</v>
@@ -27130,7 +27122,7 @@
         <v>335</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G150" s="2" t="s">
         <v>290</v>
@@ -27291,7 +27283,7 @@
         <v>336</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G151" s="2" t="s">
         <v>289</v>
@@ -27469,10 +27461,10 @@
         <v>363</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>370</v>
@@ -29781,7 +29773,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -29808,7 +29800,7 @@
         <v>283</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="C2" s="30" t="s">
         <v>405</v>
@@ -29819,7 +29811,7 @@
         <v>406</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>441</v>
+        <v>459</v>
       </c>
       <c r="C3" s="31" t="s">
         <v>407</v>
@@ -29852,7 +29844,7 @@
         <v>412</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="C6" s="31" t="s">
         <v>413</v>
@@ -29896,7 +29888,7 @@
         <v>151</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>420</v>
@@ -29907,7 +29899,7 @@
         <v>153</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>421</v>
@@ -29918,7 +29910,7 @@
         <v>161</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C12" s="31" t="s">
         <v>422</v>
@@ -29951,7 +29943,7 @@
         <v>428</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="C15" s="31" t="s">
         <v>429</v>
@@ -29962,7 +29954,7 @@
         <v>219</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C16" s="31" t="s">
         <v>430</v>
@@ -30003,10 +29995,10 @@
     </row>
     <row r="20" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A20" s="31" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C20" s="31" t="s">
         <v>439</v>
@@ -30014,10 +30006,10 @@
     </row>
     <row r="21" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="32" t="s">
+        <v>446</v>
+      </c>
+      <c r="B21" s="32" t="s">
         <v>447</v>
-      </c>
-      <c r="B21" s="32" t="s">
-        <v>448</v>
       </c>
       <c r="C21" s="31" t="s">
         <v>439</v>
@@ -30040,12 +30032,12 @@
   <sheetData>
     <row r="1" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="35" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="33" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="33" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Fixed last bug and errors for WLD.
</commit_message>
<xml_diff>
--- a/inst/extdata/Exemplar_Table.xlsx
+++ b/inst/extdata/Exemplar_Table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/Dropbox/Fellowship 1960-2015 PFU database/Database plan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/SEAPSUTWorkflow/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBDDC56-3500-9546-894C-9DBB685F4134}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE6FBC6-AE50-1445-BC99-AB383C792E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="48280" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10026" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10026" uniqueCount="479">
   <si>
     <t>Albania</t>
   </si>
@@ -1461,6 +1461,9 @@
   </si>
   <si>
     <t>FEB</t>
+  </si>
+  <si>
+    <t>WLD</t>
   </si>
 </sst>
 </file>
@@ -2233,6 +2236,9 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2286,9 +2292,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3148,7 +3151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BM153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H150" sqref="H150:BM150"/>
     </sheetView>
@@ -31803,178 +31806,178 @@
         <v>289</v>
       </c>
       <c r="H150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="J150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="K150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="L150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="M150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="N150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="O150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="P150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="Q150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="R150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="S150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="T150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="U150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="V150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="W150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="X150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="Y150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="Z150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AA150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AB150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AC150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AD150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AE150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AF150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AG150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AH150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AI150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AJ150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AK150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AL150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AM150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AN150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AO150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AP150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AQ150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AR150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AS150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AT150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AU150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AV150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AW150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AX150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AY150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="AZ150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="BA150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="BB150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="BC150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="BD150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="BE150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="BF150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="BG150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="BH150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="BI150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="BJ150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="BK150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="BL150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
       <c r="BM150" s="1" t="s">
-        <v>289</v>
+        <v>478</v>
       </c>
     </row>
     <row r="151" spans="1:65" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -34579,18 +34582,18 @@
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="45"/>
-      <c r="H3" s="52" t="s">
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="46"/>
+      <c r="H3" s="53" t="s">
         <v>372</v>
       </c>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="55"/>
       <c r="N3" s="2" t="s">
         <v>282</v>
       </c>
@@ -34602,14 +34605,14 @@
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B4" s="46"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="48"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="57"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="49"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="58"/>
       <c r="N4" s="2" t="s">
         <v>284</v>
       </c>
@@ -34621,14 +34624,14 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="49"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="51"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="60"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="52"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="61"/>
       <c r="N5" s="2" t="s">
         <v>285</v>
       </c>
@@ -34670,38 +34673,38 @@
     </row>
     <row r="8" spans="2:16" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="9" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="45"/>
-      <c r="H9" s="52" t="s">
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="46"/>
+      <c r="H9" s="53" t="s">
         <v>374</v>
       </c>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="55"/>
     </row>
     <row r="10" spans="2:16" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="46"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="48"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="57"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="49"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="58"/>
     </row>
     <row r="11" spans="2:16" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="49"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="51"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
-      <c r="K11" s="60"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="52"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="61"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B12" s="19"/>
@@ -34731,42 +34734,42 @@
       <c r="C15" s="62"/>
       <c r="D15" s="62"/>
       <c r="E15" s="62"/>
-      <c r="H15" s="52" t="s">
+      <c r="H15" s="53" t="s">
         <v>378</v>
       </c>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="54"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="55"/>
     </row>
     <row r="16" spans="2:16" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="H16" s="55"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="57"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="58"/>
     </row>
     <row r="17" spans="2:11" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="44" t="s">
         <v>381</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="45"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="60"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="46"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="60"/>
+      <c r="K17" s="61"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B18" s="46"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="48"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="49"/>
     </row>
     <row r="19" spans="2:11" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="49"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="51"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="52"/>
       <c r="H19" t="s">
         <v>376</v>
       </c>
@@ -34776,109 +34779,114 @@
       <c r="B21" t="s">
         <v>382</v>
       </c>
-      <c r="H21" s="52" t="s">
+      <c r="H21" s="53" t="s">
         <v>377</v>
       </c>
-      <c r="I21" s="53"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="54"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="55"/>
     </row>
     <row r="22" spans="2:11" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="H22" s="55"/>
-      <c r="I22" s="56"/>
-      <c r="J22" s="56"/>
-      <c r="K22" s="57"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="58"/>
     </row>
     <row r="23" spans="2:11" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="44" t="s">
         <v>383</v>
       </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="45"/>
-      <c r="H23" s="58"/>
-      <c r="I23" s="59"/>
-      <c r="J23" s="59"/>
-      <c r="K23" s="60"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="46"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="61"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B24" s="46"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="48"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="49"/>
     </row>
     <row r="25" spans="2:11" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="49"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="51"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="52"/>
       <c r="H25" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B27" s="61" t="s">
+      <c r="B27" s="43" t="s">
         <v>384</v>
       </c>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B28" s="61"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="61"/>
-      <c r="E28" s="61"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B29" s="61"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="61"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B31" s="61" t="s">
+      <c r="B31" s="43" t="s">
         <v>385</v>
       </c>
-      <c r="C31" s="61"/>
-      <c r="D31" s="61"/>
-      <c r="E31" s="61"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B32" s="61"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="61"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B33" s="61"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
     </row>
     <row r="34" spans="2:5" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="44" t="s">
         <v>386</v>
       </c>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="45"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="46"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B36" s="46"/>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="48"/>
+      <c r="B36" s="47"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="49"/>
     </row>
     <row r="37" spans="2:5" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="49"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="51"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B3:E5"/>
+    <mergeCell ref="B9:E11"/>
+    <mergeCell ref="H3:K5"/>
+    <mergeCell ref="H9:K11"/>
+    <mergeCell ref="B27:E29"/>
     <mergeCell ref="B31:E33"/>
     <mergeCell ref="B35:E37"/>
     <mergeCell ref="H15:K17"/>
@@ -34886,11 +34894,6 @@
     <mergeCell ref="B13:E15"/>
     <mergeCell ref="B17:E19"/>
     <mergeCell ref="B23:E25"/>
-    <mergeCell ref="B3:E5"/>
-    <mergeCell ref="B9:E11"/>
-    <mergeCell ref="H3:K5"/>
-    <mergeCell ref="H9:K11"/>
-    <mergeCell ref="B27:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -35424,9 +35427,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -35576,26 +35582,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83F7A5DA-1B98-4A64-9D1E-26B3B73D80C1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828852AD-0200-491F-83D2-C0A0FDC8BB33}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="77d41baf-5ecc-4842-ba36-0ed33caf7049"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -35619,9 +35614,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828852AD-0200-491F-83D2-C0A0FDC8BB33}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83F7A5DA-1B98-4A64-9D1E-26B3B73D80C1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="77d41baf-5ecc-4842-ba36-0ed33caf7049"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>